<commit_message>
- Updated data constraint
</commit_message>
<xml_diff>
--- a/B-DOCUMENT/B-API_DOCUMENTATION/data_constraints.xlsx
+++ b/B-DOCUMENT/B-API_DOCUMENTATION/data_constraints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Fields</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Regex</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>^\w+([-+.']\w+)*@\w+([-.]\w+)*\.\w+([-.]\w+)*$</t>
   </si>
   <si>
@@ -47,6 +44,61 @@
   </si>
   <si>
     <t>pagination[records]</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>^[A-Za-z0-9!@#$%^&amp;*]*$</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>- Password can contain alphanumeric
+- Password can contains special characters : !@#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>nickname</t>
+  </si>
+  <si>
+    <t>^[A-Za-z0-9]*$</t>
+  </si>
+  <si>
+    <t>- Name can contain alphanumeric</t>
+  </si>
+  <si>
+    <t>created</t>
+  </si>
+  <si>
+    <t>lastModified</t>
+  </si>
+  <si>
+    <t>joined</t>
+  </si>
+  <si>
+    <t>comment[content]</t>
+  </si>
+  <si>
+    <t>post[title]</t>
+  </si>
+  <si>
+    <t>post[body]</t>
+  </si>
+  <si>
+    <t>account[status]</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0: Disabled
+1: Pending
+2: Active
+</t>
+  </si>
+  <si>
+    <t>connection[index]</t>
   </si>
 </sst>
 </file>
@@ -82,16 +134,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -130,16 +188,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G18" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:G18"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H18" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H18"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Fields" dataDxfId="7"/>
     <tableColumn id="2" name="Min length" dataDxfId="6"/>
     <tableColumn id="3" name="Max length" dataDxfId="5"/>
     <tableColumn id="4" name="Min" dataDxfId="4"/>
     <tableColumn id="5" name="Max" dataDxfId="3"/>
     <tableColumn id="6" name="Regex" dataDxfId="2"/>
-    <tableColumn id="8" name="Other" dataDxfId="1"/>
+    <tableColumn id="8" name="Note" dataDxfId="1"/>
+    <tableColumn id="7" name="Range" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -432,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +504,11 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="49.140625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="7" max="7" width="61" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,12 +528,15 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -484,13 +547,14 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -500,10 +564,11 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -515,98 +580,171 @@
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1">
+        <v>64</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>-25200000</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>-25200000</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>-25200000</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>32</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1">
+        <v>512</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1">
+        <v>512</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="H13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1">
+        <v>36</v>
+      </c>
+      <c r="C14" s="1">
+        <v>36</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -614,8 +752,9 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -623,8 +762,9 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -632,8 +772,9 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -641,6 +782,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Added token http message.
</commit_message>
<xml_diff>
--- a/B-DOCUMENT/B-API_DOCUMENTATION/data_constraints.xlsx
+++ b/B-DOCUMENT/B-API_DOCUMENTATION/data_constraints.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Fields</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>account[nickname]</t>
+  </si>
+  <si>
+    <t>category[name]</t>
+  </si>
+  <si>
+    <t>(?=.*?[a-zA-Z]+.*?)(.*)</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,12 +751,20 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>64</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>

</xml_diff>